<commit_message>
Misc updates - mostly so MASTER excel can be read in directly from UCSRB server
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Habitat_Quality_and_Geomorphic_Potential_Rating_Criteria.xlsx
+++ b/Data/Criteria_and_Scoring/Habitat_Quality_and_Geomorphic_Potential_Rating_Criteria.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FE0F8E-E439-4C5C-AA8A-5B4717786418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108451A2-11BA-4F02-85F0-AF9ABAF5E511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="84" yWindow="4932" windowWidth="22836" windowHeight="7452" xr2:uid="{DB26C65F-EA9F-4F0C-ADCD-2FA76DCAC294}"/>
+    <workbookView xWindow="2100" yWindow="1035" windowWidth="23040" windowHeight="11385" xr2:uid="{DB26C65F-EA9F-4F0C-ADCD-2FA76DCAC294}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$122</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="229">
   <si>
     <t>Habitat_Type</t>
   </si>
@@ -621,12 +621,6 @@
     <t>Boulder_UCSRB_pct,SubEstBldr_CHAMP</t>
   </si>
   <si>
-    <t>0 - 2%</t>
-  </si>
-  <si>
-    <t>2-5%</t>
-  </si>
-  <si>
     <t>&gt;5% boulder</t>
   </si>
   <si>
@@ -745,6 +739,9 @@
   </si>
   <si>
     <t>no data present</t>
+  </si>
+  <si>
+    <t>&gt;0% and &lt;5%</t>
   </si>
 </sst>
 </file>
@@ -1167,25 +1164,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD9FED94-E706-4D30-A34B-0903E7C0B572}">
   <dimension ref="A1:T122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F135" sqref="F135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="7" width="36.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
-    <col min="10" max="10" width="24.109375" customWidth="1"/>
-    <col min="11" max="11" width="23.21875" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="7" width="36.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
+    <col min="13" max="14" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1232,7 +1230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1279,7 +1277,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1326,7 +1324,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1373,7 +1371,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1420,7 +1418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1467,7 +1465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1515,7 +1513,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1563,7 +1561,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1610,7 +1608,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1658,7 +1656,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -1684,7 +1682,7 @@
         <v>38</v>
       </c>
       <c r="I11" s="3">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="J11" s="3">
         <v>-5</v>
@@ -1705,7 +1703,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -1731,7 +1729,7 @@
         <v>38</v>
       </c>
       <c r="I12" s="3">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J12" s="3">
         <v>14</v>
@@ -1752,7 +1750,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -1800,7 +1798,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -1847,7 +1845,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -1894,7 +1892,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1941,7 +1939,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1988,7 +1986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2035,7 +2033,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2082,7 +2080,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2129,7 +2127,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2176,7 +2174,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2223,7 +2221,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -2270,7 +2268,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -2302,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="K24" s="3">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="L24" s="3">
         <v>3</v>
@@ -2317,7 +2315,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -2346,7 +2344,7 @@
         <v>4</v>
       </c>
       <c r="J25" s="3">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="K25" s="3">
         <v>5.0999999999999996</v>
@@ -2364,7 +2362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>50</v>
       </c>
@@ -2402,7 +2400,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>50</v>
       </c>
@@ -2440,7 +2438,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
@@ -2478,7 +2476,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2519,7 +2517,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>60</v>
       </c>
@@ -2562,7 +2560,7 @@
       </c>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>60</v>
       </c>
@@ -2605,7 +2603,7 @@
       </c>
       <c r="O31" s="3"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -2650,7 +2648,7 @@
       </c>
       <c r="O32" s="3"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>65</v>
       </c>
@@ -2700,7 +2698,7 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>65</v>
       </c>
@@ -2750,7 +2748,7 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>65</v>
       </c>
@@ -2802,7 +2800,7 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>73</v>
       </c>
@@ -2852,7 +2850,7 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>73</v>
       </c>
@@ -2902,7 +2900,7 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
@@ -2952,7 +2950,7 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>73</v>
       </c>
@@ -3004,7 +3002,7 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>12</v>
       </c>
@@ -3056,7 +3054,7 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>12</v>
       </c>
@@ -3108,7 +3106,7 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
@@ -3160,7 +3158,7 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>12</v>
       </c>
@@ -3212,7 +3210,7 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -3244,7 +3242,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="3">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="L44" s="6">
         <v>5</v>
@@ -3260,7 +3258,7 @@
       </c>
       <c r="Q44" s="3"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -3289,10 +3287,10 @@
         <v>18</v>
       </c>
       <c r="J45" s="3">
-        <v>0.01</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K45" s="3">
-        <v>1E-4</v>
+        <v>0.5</v>
       </c>
       <c r="L45" s="6">
         <v>3</v>
@@ -3308,7 +3306,7 @@
       </c>
       <c r="Q45" s="3"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -3340,7 +3338,7 @@
         <v>0.5</v>
       </c>
       <c r="K46" s="3">
-        <v>49.9</v>
+        <v>2</v>
       </c>
       <c r="L46" s="6">
         <v>1</v>
@@ -3356,7 +3354,7 @@
       </c>
       <c r="Q46" s="3"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -3404,7 +3402,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -3452,7 +3450,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -3500,7 +3498,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>110</v>
       </c>
@@ -3548,7 +3546,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>110</v>
       </c>
@@ -3595,7 +3593,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -3643,7 +3641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>110</v>
       </c>
@@ -3691,7 +3689,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>110</v>
       </c>
@@ -3739,7 +3737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>110</v>
       </c>
@@ -3787,7 +3785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>122</v>
       </c>
@@ -3835,7 +3833,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>122</v>
       </c>
@@ -3883,7 +3881,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>122</v>
       </c>
@@ -3931,7 +3929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>129</v>
       </c>
@@ -3960,11 +3958,10 @@
         <v>0</v>
       </c>
       <c r="J59" s="3">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K59" s="3">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="L59" s="4">
         <v>1</v>
@@ -3979,7 +3976,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>129</v>
       </c>
@@ -4008,7 +4005,7 @@
         <v>0.1</v>
       </c>
       <c r="J60" s="3">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="K60" s="3">
         <v>20</v>
@@ -4026,7 +4023,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>129</v>
       </c>
@@ -4074,7 +4071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>136</v>
       </c>
@@ -4122,7 +4119,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>136</v>
       </c>
@@ -4170,7 +4167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>136</v>
       </c>
@@ -4218,7 +4215,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>141</v>
       </c>
@@ -4266,7 +4263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>141</v>
       </c>
@@ -4314,7 +4311,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>141</v>
       </c>
@@ -4362,7 +4359,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>147</v>
       </c>
@@ -4411,7 +4408,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>147</v>
       </c>
@@ -4460,7 +4457,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>147</v>
       </c>
@@ -4509,7 +4506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>147</v>
       </c>
@@ -4559,7 +4556,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>147</v>
       </c>
@@ -4609,7 +4606,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>147</v>
       </c>
@@ -4657,7 +4654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>147</v>
       </c>
@@ -4707,7 +4704,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>147</v>
       </c>
@@ -4757,7 +4754,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>147</v>
       </c>
@@ -4807,7 +4804,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>147</v>
       </c>
@@ -4857,7 +4854,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>147</v>
       </c>
@@ -4907,7 +4904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>147</v>
       </c>
@@ -4957,7 +4954,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>147</v>
       </c>
@@ -5007,7 +5004,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>147</v>
       </c>
@@ -5057,7 +5054,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>147</v>
       </c>
@@ -5107,7 +5104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>147</v>
       </c>
@@ -5157,7 +5154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>147</v>
       </c>
@@ -5207,7 +5204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>147</v>
       </c>
@@ -5257,7 +5254,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>147</v>
       </c>
@@ -5307,7 +5304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>147</v>
       </c>
@@ -5357,7 +5354,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>147</v>
       </c>
@@ -5407,7 +5404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>147</v>
       </c>
@@ -5456,7 +5453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>147</v>
       </c>
@@ -5505,7 +5502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>147</v>
       </c>
@@ -5554,7 +5551,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>174</v>
       </c>
@@ -5597,7 +5594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>174</v>
       </c>
@@ -5639,7 +5636,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>174</v>
       </c>
@@ -5681,7 +5678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>177</v>
       </c>
@@ -5729,7 +5726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -5777,7 +5774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>177</v>
       </c>
@@ -5825,7 +5822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>184</v>
       </c>
@@ -5857,13 +5854,13 @@
         <v>-0.1</v>
       </c>
       <c r="K98" s="3">
-        <v>2</v>
+        <v>1E-4</v>
       </c>
       <c r="L98" s="4">
         <v>1</v>
       </c>
-      <c r="M98" s="14" t="s">
-        <v>188</v>
+      <c r="M98" s="14">
+        <v>0</v>
       </c>
       <c r="N98" s="3" t="s">
         <v>20</v>
@@ -5872,7 +5869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>184</v>
       </c>
@@ -5901,17 +5898,16 @@
         <v>2</v>
       </c>
       <c r="J99" s="3">
-        <f t="shared" ref="J99:J100" si="5">I99</f>
-        <v>2</v>
+        <v>1E-4</v>
       </c>
       <c r="K99" s="3">
-        <v>5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="L99" s="4">
         <v>3</v>
       </c>
       <c r="M99" s="7" t="s">
-        <v>189</v>
+        <v>228</v>
       </c>
       <c r="N99" s="3" t="s">
         <v>19</v>
@@ -5920,7 +5916,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>184</v>
       </c>
@@ -5949,8 +5945,7 @@
         <v>5</v>
       </c>
       <c r="J100" s="3">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="K100" s="3">
         <v>101</v>
@@ -5959,7 +5954,7 @@
         <v>5</v>
       </c>
       <c r="M100" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N100" s="3" t="s">
         <v>17</v>
@@ -5968,18 +5963,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B101" t="s">
         <v>185</v>
       </c>
       <c r="C101" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D101" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E101" t="s">
         <v>18</v>
@@ -6015,18 +6010,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B102" t="s">
         <v>185</v>
       </c>
       <c r="C102" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D102" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E102" t="s">
         <v>18</v>
@@ -6053,7 +6048,7 @@
         <v>3</v>
       </c>
       <c r="M102" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="N102" s="3" t="s">
         <v>19</v>
@@ -6062,18 +6057,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B103" t="s">
         <v>185</v>
       </c>
       <c r="C103" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D103" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E103" t="s">
         <v>18</v>
@@ -6091,7 +6086,7 @@
         <v>50</v>
       </c>
       <c r="J103" s="3">
-        <f t="shared" ref="J103" si="6">I103</f>
+        <f t="shared" ref="J103" si="5">I103</f>
         <v>50</v>
       </c>
       <c r="K103" s="3">
@@ -6101,7 +6096,7 @@
         <v>5</v>
       </c>
       <c r="M103" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N103" s="3" t="s">
         <v>17</v>
@@ -6110,18 +6105,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B104" t="s">
         <v>185</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D104" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E104" t="s">
         <v>18</v>
@@ -6148,7 +6143,7 @@
         <v>5</v>
       </c>
       <c r="M104" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="N104" s="3" t="s">
         <v>17</v>
@@ -6157,18 +6152,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B105" t="s">
         <v>185</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D105" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E105" t="s">
         <v>18</v>
@@ -6186,7 +6181,7 @@
         <v>12</v>
       </c>
       <c r="J105" s="3">
-        <f t="shared" ref="J105:J106" si="7">I105</f>
+        <f t="shared" ref="J105:J106" si="6">I105</f>
         <v>12</v>
       </c>
       <c r="K105" s="3">
@@ -6196,7 +6191,7 @@
         <v>3</v>
       </c>
       <c r="M105" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="N105" s="3" t="s">
         <v>19</v>
@@ -6205,18 +6200,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B106" t="s">
         <v>185</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D106" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E106" t="s">
         <v>18</v>
@@ -6234,152 +6229,152 @@
         <v>20</v>
       </c>
       <c r="J106" s="3">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K106" s="3">
+        <v>101</v>
+      </c>
+      <c r="L106" s="4">
+        <v>1</v>
+      </c>
+      <c r="M106" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="N106" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O106" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>200</v>
+      </c>
+      <c r="B107" t="s">
+        <v>185</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D107" t="s">
+        <v>201</v>
+      </c>
+      <c r="E107" t="s">
+        <v>18</v>
+      </c>
+      <c r="F107" t="s">
+        <v>18</v>
+      </c>
+      <c r="G107" t="s">
+        <v>18</v>
+      </c>
+      <c r="H107" t="s">
+        <v>38</v>
+      </c>
+      <c r="I107" s="3">
+        <v>0</v>
+      </c>
+      <c r="J107" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="K107" s="3">
+        <v>10</v>
+      </c>
+      <c r="L107" s="4">
+        <v>1</v>
+      </c>
+      <c r="M107" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="N107" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O107" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>200</v>
+      </c>
+      <c r="B108" t="s">
+        <v>185</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D108" t="s">
+        <v>201</v>
+      </c>
+      <c r="E108" t="s">
+        <v>18</v>
+      </c>
+      <c r="F108" t="s">
+        <v>18</v>
+      </c>
+      <c r="G108" t="s">
+        <v>18</v>
+      </c>
+      <c r="H108" t="s">
+        <v>38</v>
+      </c>
+      <c r="I108" s="3">
+        <v>10</v>
+      </c>
+      <c r="J108" s="3">
+        <f t="shared" ref="J108:J109" si="7">I108</f>
+        <v>10</v>
+      </c>
+      <c r="K108" s="3">
+        <v>20</v>
+      </c>
+      <c r="L108" s="4">
+        <v>3</v>
+      </c>
+      <c r="M108" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="N108" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O108" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>200</v>
+      </c>
+      <c r="B109" t="s">
+        <v>185</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D109" t="s">
+        <v>201</v>
+      </c>
+      <c r="E109" t="s">
+        <v>18</v>
+      </c>
+      <c r="F109" t="s">
+        <v>18</v>
+      </c>
+      <c r="G109" t="s">
+        <v>18</v>
+      </c>
+      <c r="H109" t="s">
+        <v>38</v>
+      </c>
+      <c r="I109" s="3">
+        <v>20</v>
+      </c>
+      <c r="J109" s="3">
         <f t="shared" si="7"/>
         <v>20</v>
       </c>
-      <c r="K106" s="3">
-        <v>101</v>
-      </c>
-      <c r="L106" s="4">
-        <v>1</v>
-      </c>
-      <c r="M106" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="N106" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O106" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>202</v>
-      </c>
-      <c r="B107" t="s">
-        <v>185</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D107" t="s">
-        <v>203</v>
-      </c>
-      <c r="E107" t="s">
-        <v>18</v>
-      </c>
-      <c r="F107" t="s">
-        <v>18</v>
-      </c>
-      <c r="G107" t="s">
-        <v>18</v>
-      </c>
-      <c r="H107" t="s">
-        <v>38</v>
-      </c>
-      <c r="I107" s="3">
-        <v>0</v>
-      </c>
-      <c r="J107" s="3">
-        <v>-0.1</v>
-      </c>
-      <c r="K107" s="3">
-        <v>10</v>
-      </c>
-      <c r="L107" s="4">
-        <v>1</v>
-      </c>
-      <c r="M107" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="N107" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O107" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>202</v>
-      </c>
-      <c r="B108" t="s">
-        <v>185</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D108" t="s">
-        <v>203</v>
-      </c>
-      <c r="E108" t="s">
-        <v>18</v>
-      </c>
-      <c r="F108" t="s">
-        <v>18</v>
-      </c>
-      <c r="G108" t="s">
-        <v>18</v>
-      </c>
-      <c r="H108" t="s">
-        <v>38</v>
-      </c>
-      <c r="I108" s="3">
-        <v>10</v>
-      </c>
-      <c r="J108" s="3">
-        <f t="shared" ref="J108:J109" si="8">I108</f>
-        <v>10</v>
-      </c>
-      <c r="K108" s="3">
-        <v>20</v>
-      </c>
-      <c r="L108" s="4">
-        <v>3</v>
-      </c>
-      <c r="M108" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="N108" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O108" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>202</v>
-      </c>
-      <c r="B109" t="s">
-        <v>185</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D109" t="s">
-        <v>203</v>
-      </c>
-      <c r="E109" t="s">
-        <v>18</v>
-      </c>
-      <c r="F109" t="s">
-        <v>18</v>
-      </c>
-      <c r="G109" t="s">
-        <v>18</v>
-      </c>
-      <c r="H109" t="s">
-        <v>38</v>
-      </c>
-      <c r="I109" s="3">
-        <v>20</v>
-      </c>
-      <c r="J109" s="3">
-        <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
       <c r="K109" s="3">
         <v>100000</v>
       </c>
@@ -6387,7 +6382,7 @@
         <v>5</v>
       </c>
       <c r="M109" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="N109" s="3" t="s">
         <v>17</v>
@@ -6396,18 +6391,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B110" t="s">
         <v>185</v>
       </c>
       <c r="C110" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D110" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E110" t="s">
         <v>18</v>
@@ -6434,7 +6429,7 @@
         <v>5</v>
       </c>
       <c r="M110" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N110" s="3" t="s">
         <v>17</v>
@@ -6443,18 +6438,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B111" t="s">
         <v>185</v>
       </c>
       <c r="C111" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D111" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E111" t="s">
         <v>18</v>
@@ -6472,7 +6467,7 @@
         <v>15</v>
       </c>
       <c r="J111" s="3">
-        <f t="shared" ref="J111:J112" si="9">I111</f>
+        <f t="shared" ref="J111:J112" si="8">I111</f>
         <v>15</v>
       </c>
       <c r="K111" s="3">
@@ -6482,7 +6477,7 @@
         <v>3</v>
       </c>
       <c r="M111" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N111" s="3" t="s">
         <v>19</v>
@@ -6491,18 +6486,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B112" t="s">
         <v>185</v>
       </c>
       <c r="C112" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D112" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E112" t="s">
         <v>18</v>
@@ -6520,7 +6515,7 @@
         <v>30</v>
       </c>
       <c r="J112" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
       <c r="K112" s="3">
@@ -6530,7 +6525,7 @@
         <v>1</v>
       </c>
       <c r="M112" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="N112" s="3" t="s">
         <v>20</v>
@@ -6539,18 +6534,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B113" t="s">
         <v>185</v>
       </c>
       <c r="C113" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D113" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E113" t="s">
         <v>18</v>
@@ -6577,27 +6572,27 @@
         <v>1</v>
       </c>
       <c r="M113" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="N113" s="3" t="s">
         <v>20</v>
       </c>
       <c r="O113" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B114" t="s">
         <v>185</v>
       </c>
       <c r="C114" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D114" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E114" t="s">
         <v>18</v>
@@ -6624,27 +6619,27 @@
         <v>3</v>
       </c>
       <c r="M114" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N114" s="3" t="s">
         <v>19</v>
       </c>
       <c r="O114" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B115" t="s">
         <v>185</v>
       </c>
       <c r="C115" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D115" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E115" t="s">
         <v>18</v>
@@ -6671,24 +6666,24 @@
         <v>5</v>
       </c>
       <c r="M115" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N115" s="3" t="s">
         <v>17</v>
       </c>
       <c r="O115" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B116" t="s">
         <v>24</v>
       </c>
       <c r="D116" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E116" t="s">
         <v>18</v>
@@ -6703,7 +6698,7 @@
         <v>16</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J116" s="3" t="s">
         <v>18</v>
@@ -6715,7 +6710,7 @@
         <v>1</v>
       </c>
       <c r="M116" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="N116" s="3" t="s">
         <v>18</v>
@@ -6724,15 +6719,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B117" t="s">
         <v>24</v>
       </c>
       <c r="D117" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E117" t="s">
         <v>18</v>
@@ -6747,7 +6742,7 @@
         <v>16</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J117" s="3" t="s">
         <v>18</v>
@@ -6759,7 +6754,7 @@
         <v>3</v>
       </c>
       <c r="M117" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="N117" s="3" t="s">
         <v>18</v>
@@ -6768,15 +6763,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B118" t="s">
         <v>24</v>
       </c>
       <c r="D118" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E118" t="s">
         <v>18</v>
@@ -6791,7 +6786,7 @@
         <v>16</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J118" s="3" t="s">
         <v>18</v>
@@ -6812,9 +6807,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B119" t="s">
         <v>36</v>
@@ -6823,7 +6818,7 @@
         <v>13</v>
       </c>
       <c r="D119" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E119" t="s">
         <v>18</v>
@@ -6850,7 +6845,7 @@
         <v>5</v>
       </c>
       <c r="M119" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="N119" s="3" t="s">
         <v>17</v>
@@ -6859,9 +6854,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B120" t="s">
         <v>36</v>
@@ -6870,7 +6865,7 @@
         <v>13</v>
       </c>
       <c r="D120" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E120" t="s">
         <v>18</v>
@@ -6897,7 +6892,7 @@
         <v>3</v>
       </c>
       <c r="M120" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N120" s="3" t="s">
         <v>19</v>
@@ -6906,9 +6901,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B121" t="s">
         <v>36</v>
@@ -6917,7 +6912,7 @@
         <v>13</v>
       </c>
       <c r="D121" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E121" t="s">
         <v>18</v>
@@ -6944,7 +6939,7 @@
         <v>1</v>
       </c>
       <c r="M121" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="N121" s="3" t="s">
         <v>20</v>
@@ -6953,9 +6948,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B122" t="s">
         <v>36</v>
@@ -6964,7 +6959,7 @@
         <v>13</v>
       </c>
       <c r="D122" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E122" t="s">
         <v>18</v>
@@ -6991,7 +6986,7 @@
         <v>18</v>
       </c>
       <c r="M122" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="N122" s="3" t="s">
         <v>18</v>
@@ -7001,7 +6996,19 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O46" xr:uid="{1E9C2260-2CB8-447D-8A92-7DAF23E0141C}"/>
+  <autoFilter ref="A1:O122" xr:uid="{1E9C2260-2CB8-447D-8A92-7DAF23E0141C}"/>
+  <conditionalFormatting sqref="L2:L122">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O7" r:id="rId1" xr:uid="{2507E6E6-3B57-4499-BD80-145649B4E2CC}"/>
     <hyperlink ref="O8" r:id="rId2" xr:uid="{0E31C8E0-3733-4D4D-8C84-E6B3F33AA069}"/>

</xml_diff>

<commit_message>
Updating code so Okanogan habitat data can be utilized
Not completely done, wanted to commit and push changes so they get saved remotely
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Habitat_Quality_and_Geomorphic_Potential_Rating_Criteria.xlsx
+++ b/Data/Criteria_and_Scoring/Habitat_Quality_and_Geomorphic_Potential_Rating_Criteria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE45A02-B050-4FFE-B6B4-D3134D7E4893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF2F551-F68D-44F0-A464-E93789ABCAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="20208" windowHeight="10320" xr2:uid="{DB26C65F-EA9F-4F0C-ADCD-2FA76DCAC294}"/>
+    <workbookView xWindow="-19335" yWindow="-16035" windowWidth="27960" windowHeight="15000" xr2:uid="{DB26C65F-EA9F-4F0C-ADCD-2FA76DCAC294}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="235">
   <si>
     <t>Habitat_Type</t>
   </si>
@@ -742,6 +742,24 @@
   </si>
   <si>
     <t>Floodplain Connectivity</t>
+  </si>
+  <si>
+    <t>CCT_OBMEP_embeddedness</t>
+  </si>
+  <si>
+    <t>CCT_OBMEP_fines_and_sands</t>
+  </si>
+  <si>
+    <t>CCT_OBMEP_gravel_and_small_cobbles</t>
+  </si>
+  <si>
+    <t>CCT_OBMEP_LWM_pieces_per_mile</t>
+  </si>
+  <si>
+    <t>CCT_OBMEP_channel_type_side_channel_and_off_channel_PRCNT</t>
+  </si>
+  <si>
+    <t>CCT_OBMEP_pools_per_mile</t>
   </si>
 </sst>
 </file>
@@ -1162,28 +1180,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD9FED94-E706-4D30-A34B-0903E7C0B572}">
-  <dimension ref="A1:T122"/>
+  <dimension ref="A1:T164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C123" sqref="C123"/>
+      <selection pane="bottomLeft" activeCell="F166" sqref="F166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="7" width="36.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="24.109375" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" customWidth="1"/>
-    <col min="13" max="14" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="7" width="36.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
+    <col min="13" max="14" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1230,7 +1248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1277,7 +1295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1324,7 +1342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1371,7 +1389,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1418,7 +1436,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1465,7 +1483,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1513,7 +1531,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1561,7 +1579,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1608,7 +1626,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1656,7 +1674,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -1703,7 +1721,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -1750,7 +1768,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -1798,7 +1816,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -1845,7 +1863,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -1892,7 +1910,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1939,7 +1957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1986,7 +2004,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2033,7 +2051,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2080,7 +2098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2127,7 +2145,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2174,7 +2192,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2221,7 +2239,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -2268,7 +2286,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -2315,7 +2333,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -2362,7 +2380,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>50</v>
       </c>
@@ -2400,7 +2418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>50</v>
       </c>
@@ -2438,7 +2456,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
@@ -2476,7 +2494,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2517,7 +2535,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>60</v>
       </c>
@@ -2560,7 +2578,7 @@
       </c>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>60</v>
       </c>
@@ -2603,7 +2621,7 @@
       </c>
       <c r="O31" s="3"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -2648,7 +2666,7 @@
       </c>
       <c r="O32" s="3"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>65</v>
       </c>
@@ -2698,7 +2716,7 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>65</v>
       </c>
@@ -2748,7 +2766,7 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>65</v>
       </c>
@@ -2800,7 +2818,7 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>73</v>
       </c>
@@ -2850,7 +2868,7 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>73</v>
       </c>
@@ -2900,7 +2918,7 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
@@ -2950,7 +2968,7 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>73</v>
       </c>
@@ -3002,7 +3020,7 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>12</v>
       </c>
@@ -3054,7 +3072,7 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>12</v>
       </c>
@@ -3106,7 +3124,7 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
@@ -3158,7 +3176,7 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>12</v>
       </c>
@@ -3210,7 +3228,7 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -3258,7 +3276,7 @@
       </c>
       <c r="Q44" s="3"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -3306,7 +3324,7 @@
       </c>
       <c r="Q45" s="3"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -3354,7 +3372,7 @@
       </c>
       <c r="Q46" s="3"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -3402,7 +3420,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -3450,7 +3468,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -3498,7 +3516,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>109</v>
       </c>
@@ -3546,7 +3564,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>109</v>
       </c>
@@ -3593,7 +3611,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>109</v>
       </c>
@@ -3641,7 +3659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -3689,7 +3707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -3737,7 +3755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -3785,7 +3803,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>121</v>
       </c>
@@ -3833,7 +3851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -3881,7 +3899,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>121</v>
       </c>
@@ -3929,7 +3947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>128</v>
       </c>
@@ -3976,7 +3994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>128</v>
       </c>
@@ -4023,7 +4041,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>128</v>
       </c>
@@ -4071,7 +4089,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>135</v>
       </c>
@@ -4119,7 +4137,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>135</v>
       </c>
@@ -4167,7 +4185,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -4215,7 +4233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>140</v>
       </c>
@@ -4263,7 +4281,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>140</v>
       </c>
@@ -4311,7 +4329,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>140</v>
       </c>
@@ -4359,7 +4377,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>146</v>
       </c>
@@ -4408,7 +4426,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>146</v>
       </c>
@@ -4457,7 +4475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>146</v>
       </c>
@@ -4506,7 +4524,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>146</v>
       </c>
@@ -4556,7 +4574,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>146</v>
       </c>
@@ -4606,7 +4624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>146</v>
       </c>
@@ -4654,7 +4672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>146</v>
       </c>
@@ -4704,7 +4722,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -4754,7 +4772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>146</v>
       </c>
@@ -4804,7 +4822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>146</v>
       </c>
@@ -4854,7 +4872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>146</v>
       </c>
@@ -4904,7 +4922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>146</v>
       </c>
@@ -4954,7 +4972,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>146</v>
       </c>
@@ -5004,7 +5022,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>146</v>
       </c>
@@ -5054,7 +5072,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>146</v>
       </c>
@@ -5104,7 +5122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>146</v>
       </c>
@@ -5154,7 +5172,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>146</v>
       </c>
@@ -5204,7 +5222,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>146</v>
       </c>
@@ -5254,7 +5272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>146</v>
       </c>
@@ -5304,7 +5322,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>146</v>
       </c>
@@ -5354,7 +5372,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>146</v>
       </c>
@@ -5404,7 +5422,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>146</v>
       </c>
@@ -5453,7 +5471,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>146</v>
       </c>
@@ -5502,7 +5520,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>146</v>
       </c>
@@ -5551,7 +5569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>173</v>
       </c>
@@ -5594,7 +5612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>173</v>
       </c>
@@ -5636,7 +5654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>173</v>
       </c>
@@ -5678,7 +5696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>176</v>
       </c>
@@ -5726,7 +5744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>176</v>
       </c>
@@ -5774,7 +5792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>176</v>
       </c>
@@ -5822,7 +5840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>183</v>
       </c>
@@ -5869,7 +5887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>183</v>
       </c>
@@ -5916,7 +5934,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>183</v>
       </c>
@@ -5963,7 +5981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>188</v>
       </c>
@@ -6010,7 +6028,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>188</v>
       </c>
@@ -6057,7 +6075,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>188</v>
       </c>
@@ -6105,7 +6123,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>193</v>
       </c>
@@ -6152,7 +6170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>193</v>
       </c>
@@ -6200,7 +6218,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>193</v>
       </c>
@@ -6248,7 +6266,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>199</v>
       </c>
@@ -6295,7 +6313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>199</v>
       </c>
@@ -6343,7 +6361,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>199</v>
       </c>
@@ -6391,7 +6409,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>204</v>
       </c>
@@ -6438,7 +6456,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>204</v>
       </c>
@@ -6486,7 +6504,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>204</v>
       </c>
@@ -6534,7 +6552,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>209</v>
       </c>
@@ -6581,7 +6599,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>209</v>
       </c>
@@ -6628,7 +6646,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>209</v>
       </c>
@@ -6675,7 +6693,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>215</v>
       </c>
@@ -6719,7 +6737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>215</v>
       </c>
@@ -6763,7 +6781,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>215</v>
       </c>
@@ -6807,7 +6825,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>221</v>
       </c>
@@ -6854,7 +6872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>221</v>
       </c>
@@ -6901,7 +6919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>221</v>
       </c>
@@ -6948,7 +6966,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>221</v>
       </c>
@@ -6995,9 +7013,2060 @@
         <v>18</v>
       </c>
     </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>229</v>
+      </c>
+      <c r="B123" t="s">
+        <v>184</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D123" t="s">
+        <v>229</v>
+      </c>
+      <c r="E123" t="s">
+        <v>18</v>
+      </c>
+      <c r="F123" t="s">
+        <v>18</v>
+      </c>
+      <c r="G123" t="s">
+        <v>18</v>
+      </c>
+      <c r="H123" t="s">
+        <v>38</v>
+      </c>
+      <c r="I123" s="3">
+        <v>0</v>
+      </c>
+      <c r="J123" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="K123" s="3">
+        <v>15</v>
+      </c>
+      <c r="L123" s="4">
+        <v>5</v>
+      </c>
+      <c r="M123" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="N123" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O123" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>229</v>
+      </c>
+      <c r="B124" t="s">
+        <v>184</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D124" t="s">
+        <v>229</v>
+      </c>
+      <c r="E124" t="s">
+        <v>18</v>
+      </c>
+      <c r="F124" t="s">
+        <v>18</v>
+      </c>
+      <c r="G124" t="s">
+        <v>18</v>
+      </c>
+      <c r="H124" t="s">
+        <v>38</v>
+      </c>
+      <c r="I124" s="3">
+        <v>15</v>
+      </c>
+      <c r="J124" s="3">
+        <f t="shared" ref="J124:J125" si="9">I124</f>
+        <v>15</v>
+      </c>
+      <c r="K124" s="3">
+        <v>30</v>
+      </c>
+      <c r="L124" s="4">
+        <v>3</v>
+      </c>
+      <c r="M124" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="N124" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O124" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>229</v>
+      </c>
+      <c r="B125" t="s">
+        <v>184</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D125" t="s">
+        <v>229</v>
+      </c>
+      <c r="E125" t="s">
+        <v>18</v>
+      </c>
+      <c r="F125" t="s">
+        <v>18</v>
+      </c>
+      <c r="G125" t="s">
+        <v>18</v>
+      </c>
+      <c r="H125" t="s">
+        <v>38</v>
+      </c>
+      <c r="I125" s="3">
+        <v>30</v>
+      </c>
+      <c r="J125" s="3">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="K125" s="3">
+        <v>101</v>
+      </c>
+      <c r="L125" s="4">
+        <v>1</v>
+      </c>
+      <c r="M125" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="N125" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O125" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>230</v>
+      </c>
+      <c r="B126" t="s">
+        <v>184</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D126" t="s">
+        <v>230</v>
+      </c>
+      <c r="E126" t="s">
+        <v>18</v>
+      </c>
+      <c r="F126" t="s">
+        <v>18</v>
+      </c>
+      <c r="G126" t="s">
+        <v>18</v>
+      </c>
+      <c r="H126" t="s">
+        <v>38</v>
+      </c>
+      <c r="I126" s="3">
+        <v>0</v>
+      </c>
+      <c r="J126" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="K126" s="3">
+        <v>12</v>
+      </c>
+      <c r="L126" s="4">
+        <v>5</v>
+      </c>
+      <c r="M126" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="N126" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O126" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>230</v>
+      </c>
+      <c r="B127" t="s">
+        <v>184</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D127" t="s">
+        <v>230</v>
+      </c>
+      <c r="E127" t="s">
+        <v>18</v>
+      </c>
+      <c r="F127" t="s">
+        <v>18</v>
+      </c>
+      <c r="G127" t="s">
+        <v>18</v>
+      </c>
+      <c r="H127" t="s">
+        <v>38</v>
+      </c>
+      <c r="I127" s="3">
+        <v>12</v>
+      </c>
+      <c r="J127" s="3">
+        <f t="shared" ref="J127:J128" si="10">I127</f>
+        <v>12</v>
+      </c>
+      <c r="K127" s="3">
+        <v>20</v>
+      </c>
+      <c r="L127" s="4">
+        <v>3</v>
+      </c>
+      <c r="M127" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="N127" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O127" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>230</v>
+      </c>
+      <c r="B128" t="s">
+        <v>184</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D128" t="s">
+        <v>230</v>
+      </c>
+      <c r="E128" t="s">
+        <v>18</v>
+      </c>
+      <c r="F128" t="s">
+        <v>18</v>
+      </c>
+      <c r="G128" t="s">
+        <v>18</v>
+      </c>
+      <c r="H128" t="s">
+        <v>38</v>
+      </c>
+      <c r="I128" s="3">
+        <v>20</v>
+      </c>
+      <c r="J128" s="3">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="K128" s="3">
+        <v>101</v>
+      </c>
+      <c r="L128" s="4">
+        <v>1</v>
+      </c>
+      <c r="M128" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="N128" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O128" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>231</v>
+      </c>
+      <c r="B129" t="s">
+        <v>184</v>
+      </c>
+      <c r="C129" t="s">
+        <v>189</v>
+      </c>
+      <c r="D129" t="s">
+        <v>231</v>
+      </c>
+      <c r="E129" t="s">
+        <v>18</v>
+      </c>
+      <c r="F129" t="s">
+        <v>18</v>
+      </c>
+      <c r="G129" t="s">
+        <v>18</v>
+      </c>
+      <c r="H129" t="s">
+        <v>38</v>
+      </c>
+      <c r="I129" s="3">
+        <v>0</v>
+      </c>
+      <c r="J129" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="K129" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L129" s="4">
+        <v>1</v>
+      </c>
+      <c r="M129" s="5">
+        <v>0</v>
+      </c>
+      <c r="N129" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O129" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>231</v>
+      </c>
+      <c r="B130" t="s">
+        <v>184</v>
+      </c>
+      <c r="C130" t="s">
+        <v>189</v>
+      </c>
+      <c r="D130" t="s">
+        <v>231</v>
+      </c>
+      <c r="E130" t="s">
+        <v>18</v>
+      </c>
+      <c r="F130" t="s">
+        <v>18</v>
+      </c>
+      <c r="G130" t="s">
+        <v>18</v>
+      </c>
+      <c r="H130" t="s">
+        <v>38</v>
+      </c>
+      <c r="I130" s="3">
+        <v>1</v>
+      </c>
+      <c r="J130" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K130" s="3">
+        <v>50</v>
+      </c>
+      <c r="L130" s="4">
+        <v>3</v>
+      </c>
+      <c r="M130" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="N130" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O130" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>231</v>
+      </c>
+      <c r="B131" t="s">
+        <v>184</v>
+      </c>
+      <c r="C131" t="s">
+        <v>189</v>
+      </c>
+      <c r="D131" t="s">
+        <v>231</v>
+      </c>
+      <c r="E131" t="s">
+        <v>18</v>
+      </c>
+      <c r="F131" t="s">
+        <v>18</v>
+      </c>
+      <c r="G131" t="s">
+        <v>18</v>
+      </c>
+      <c r="H131" t="s">
+        <v>38</v>
+      </c>
+      <c r="I131" s="3">
+        <v>50</v>
+      </c>
+      <c r="J131" s="3">
+        <f t="shared" ref="J131" si="11">I131</f>
+        <v>50</v>
+      </c>
+      <c r="K131" s="3">
+        <v>101</v>
+      </c>
+      <c r="L131" s="4">
+        <v>5</v>
+      </c>
+      <c r="M131" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="N131" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O131" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>232</v>
+      </c>
+      <c r="B132" t="s">
+        <v>110</v>
+      </c>
+      <c r="C132" t="s">
+        <v>111</v>
+      </c>
+      <c r="D132" t="s">
+        <v>232</v>
+      </c>
+      <c r="E132" t="s">
+        <v>113</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+      <c r="G132">
+        <v>5</v>
+      </c>
+      <c r="H132" t="s">
+        <v>38</v>
+      </c>
+      <c r="I132" s="3">
+        <v>0</v>
+      </c>
+      <c r="J132" s="3">
+        <f>I132</f>
+        <v>0</v>
+      </c>
+      <c r="K132" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L132" s="4">
+        <v>1</v>
+      </c>
+      <c r="M132" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="N132" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O132" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>232</v>
+      </c>
+      <c r="B133" t="s">
+        <v>110</v>
+      </c>
+      <c r="C133" t="s">
+        <v>111</v>
+      </c>
+      <c r="D133" t="s">
+        <v>232</v>
+      </c>
+      <c r="E133" t="s">
+        <v>113</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+      <c r="G133">
+        <v>5</v>
+      </c>
+      <c r="H133" t="s">
+        <v>38</v>
+      </c>
+      <c r="I133" s="3">
+        <v>0</v>
+      </c>
+      <c r="J133" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K133" s="3">
+        <v>20</v>
+      </c>
+      <c r="L133" s="4">
+        <v>3</v>
+      </c>
+      <c r="M133" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="N133" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O133" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>232</v>
+      </c>
+      <c r="B134" t="s">
+        <v>110</v>
+      </c>
+      <c r="C134" t="s">
+        <v>111</v>
+      </c>
+      <c r="D134" t="s">
+        <v>232</v>
+      </c>
+      <c r="E134" t="s">
+        <v>113</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
+      <c r="G134">
+        <v>5</v>
+      </c>
+      <c r="H134" t="s">
+        <v>38</v>
+      </c>
+      <c r="I134" s="3">
+        <v>20</v>
+      </c>
+      <c r="J134" s="3">
+        <f t="shared" ref="J134:J164" si="12">I134</f>
+        <v>20</v>
+      </c>
+      <c r="K134" s="3">
+        <v>100000</v>
+      </c>
+      <c r="L134" s="4">
+        <v>5</v>
+      </c>
+      <c r="M134" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="N134" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O134" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>232</v>
+      </c>
+      <c r="B135" t="s">
+        <v>110</v>
+      </c>
+      <c r="C135" t="s">
+        <v>111</v>
+      </c>
+      <c r="D135" t="s">
+        <v>232</v>
+      </c>
+      <c r="E135" t="s">
+        <v>117</v>
+      </c>
+      <c r="F135">
+        <v>5</v>
+      </c>
+      <c r="G135">
+        <v>100000</v>
+      </c>
+      <c r="H135" t="s">
+        <v>38</v>
+      </c>
+      <c r="I135" s="3">
+        <v>0</v>
+      </c>
+      <c r="J135" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K135" s="3">
+        <v>17</v>
+      </c>
+      <c r="L135" s="4">
+        <v>1</v>
+      </c>
+      <c r="M135" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N135" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O135" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>232</v>
+      </c>
+      <c r="B136" t="s">
+        <v>110</v>
+      </c>
+      <c r="C136" t="s">
+        <v>111</v>
+      </c>
+      <c r="D136" t="s">
+        <v>232</v>
+      </c>
+      <c r="E136" t="s">
+        <v>117</v>
+      </c>
+      <c r="F136">
+        <v>5</v>
+      </c>
+      <c r="G136">
+        <v>100000</v>
+      </c>
+      <c r="H136" t="s">
+        <v>38</v>
+      </c>
+      <c r="I136" s="3">
+        <v>17</v>
+      </c>
+      <c r="J136" s="3">
+        <f t="shared" si="12"/>
+        <v>17</v>
+      </c>
+      <c r="K136" s="3">
+        <v>70</v>
+      </c>
+      <c r="L136" s="4">
+        <v>3</v>
+      </c>
+      <c r="M136" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N136" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O136" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>232</v>
+      </c>
+      <c r="B137" t="s">
+        <v>110</v>
+      </c>
+      <c r="C137" t="s">
+        <v>111</v>
+      </c>
+      <c r="D137" t="s">
+        <v>232</v>
+      </c>
+      <c r="E137" t="s">
+        <v>117</v>
+      </c>
+      <c r="F137">
+        <v>5</v>
+      </c>
+      <c r="G137">
+        <v>100000</v>
+      </c>
+      <c r="H137" t="s">
+        <v>38</v>
+      </c>
+      <c r="I137" s="3">
+        <v>70</v>
+      </c>
+      <c r="J137" s="3">
+        <f t="shared" si="12"/>
+        <v>70</v>
+      </c>
+      <c r="K137" s="3">
+        <v>100000</v>
+      </c>
+      <c r="L137" s="4">
+        <v>5</v>
+      </c>
+      <c r="M137" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="N137" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O137" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>233</v>
+      </c>
+      <c r="B138" t="s">
+        <v>177</v>
+      </c>
+      <c r="C138" t="s">
+        <v>178</v>
+      </c>
+      <c r="D138" t="s">
+        <v>233</v>
+      </c>
+      <c r="E138" t="s">
+        <v>18</v>
+      </c>
+      <c r="F138" t="s">
+        <v>18</v>
+      </c>
+      <c r="G138" t="s">
+        <v>18</v>
+      </c>
+      <c r="H138" t="s">
+        <v>38</v>
+      </c>
+      <c r="I138" s="3">
+        <v>0</v>
+      </c>
+      <c r="J138" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K138" s="3">
+        <v>2</v>
+      </c>
+      <c r="L138" s="4">
+        <v>1</v>
+      </c>
+      <c r="M138" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="N138" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O138" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>233</v>
+      </c>
+      <c r="B139" t="s">
+        <v>177</v>
+      </c>
+      <c r="C139" t="s">
+        <v>178</v>
+      </c>
+      <c r="D139" t="s">
+        <v>233</v>
+      </c>
+      <c r="E139" t="s">
+        <v>18</v>
+      </c>
+      <c r="F139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G139" t="s">
+        <v>18</v>
+      </c>
+      <c r="H139" t="s">
+        <v>38</v>
+      </c>
+      <c r="I139" s="3">
+        <v>2</v>
+      </c>
+      <c r="J139" s="3">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="K139" s="3">
+        <v>5</v>
+      </c>
+      <c r="L139" s="4">
+        <v>3</v>
+      </c>
+      <c r="M139" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="N139" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O139" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>233</v>
+      </c>
+      <c r="B140" t="s">
+        <v>177</v>
+      </c>
+      <c r="C140" t="s">
+        <v>178</v>
+      </c>
+      <c r="D140" t="s">
+        <v>233</v>
+      </c>
+      <c r="E140" t="s">
+        <v>18</v>
+      </c>
+      <c r="F140" t="s">
+        <v>18</v>
+      </c>
+      <c r="G140" t="s">
+        <v>18</v>
+      </c>
+      <c r="H140" t="s">
+        <v>38</v>
+      </c>
+      <c r="I140" s="3">
+        <v>5</v>
+      </c>
+      <c r="J140" s="3">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="K140" s="3">
+        <v>101</v>
+      </c>
+      <c r="L140" s="4">
+        <v>5</v>
+      </c>
+      <c r="M140" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="N140" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O140" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>146</v>
+      </c>
+      <c r="B141" t="s">
+        <v>129</v>
+      </c>
+      <c r="C141" t="s">
+        <v>141</v>
+      </c>
+      <c r="D141" t="s">
+        <v>234</v>
+      </c>
+      <c r="E141" t="s">
+        <v>148</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+      <c r="G141">
+        <f>5*0.3048</f>
+        <v>1.524</v>
+      </c>
+      <c r="H141" t="s">
+        <v>38</v>
+      </c>
+      <c r="I141" s="3">
+        <v>0</v>
+      </c>
+      <c r="J141" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K141" s="3">
+        <v>184</v>
+      </c>
+      <c r="L141" s="4">
+        <v>1</v>
+      </c>
+      <c r="M141" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="N141" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O141" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>146</v>
+      </c>
+      <c r="B142" t="s">
+        <v>129</v>
+      </c>
+      <c r="C142" t="s">
+        <v>141</v>
+      </c>
+      <c r="D142" t="s">
+        <v>234</v>
+      </c>
+      <c r="E142" t="s">
+        <v>148</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="G142">
+        <f>5*0.3048</f>
+        <v>1.524</v>
+      </c>
+      <c r="H142" t="s">
+        <v>38</v>
+      </c>
+      <c r="I142" s="3">
+        <v>184</v>
+      </c>
+      <c r="J142" s="3">
+        <f t="shared" si="12"/>
+        <v>184</v>
+      </c>
+      <c r="K142" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L142" s="4">
+        <v>5</v>
+      </c>
+      <c r="M142" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="N142" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O142" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>146</v>
+      </c>
+      <c r="B143" t="s">
+        <v>129</v>
+      </c>
+      <c r="C143" t="s">
+        <v>141</v>
+      </c>
+      <c r="D143" t="s">
+        <v>234</v>
+      </c>
+      <c r="E143" t="s">
+        <v>148</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <f>5*0.3048</f>
+        <v>1.524</v>
+      </c>
+      <c r="H143" t="s">
+        <v>38</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J143" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="K143" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L143" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M143" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N143" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O143" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>146</v>
+      </c>
+      <c r="B144" t="s">
+        <v>129</v>
+      </c>
+      <c r="C144" t="s">
+        <v>141</v>
+      </c>
+      <c r="D144" t="s">
+        <v>234</v>
+      </c>
+      <c r="E144" t="s">
+        <v>152</v>
+      </c>
+      <c r="F144">
+        <f>5*0.3048</f>
+        <v>1.524</v>
+      </c>
+      <c r="G144">
+        <f>10*0.3048</f>
+        <v>3.048</v>
+      </c>
+      <c r="H144" t="s">
+        <v>38</v>
+      </c>
+      <c r="I144" s="3">
+        <v>0</v>
+      </c>
+      <c r="J144" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K144" s="3">
+        <v>95</v>
+      </c>
+      <c r="L144" s="4">
+        <v>1</v>
+      </c>
+      <c r="M144" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="N144" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O144" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>146</v>
+      </c>
+      <c r="B145" t="s">
+        <v>129</v>
+      </c>
+      <c r="C145" t="s">
+        <v>141</v>
+      </c>
+      <c r="D145" t="s">
+        <v>234</v>
+      </c>
+      <c r="E145" t="s">
+        <v>152</v>
+      </c>
+      <c r="F145">
+        <f>5*0.3048</f>
+        <v>1.524</v>
+      </c>
+      <c r="G145">
+        <f>10*0.3048</f>
+        <v>3.048</v>
+      </c>
+      <c r="H145" t="s">
+        <v>38</v>
+      </c>
+      <c r="I145" s="3">
+        <v>95</v>
+      </c>
+      <c r="J145" s="3">
+        <f t="shared" si="12"/>
+        <v>95</v>
+      </c>
+      <c r="K145" s="3">
+        <v>100000</v>
+      </c>
+      <c r="L145" s="4">
+        <v>5</v>
+      </c>
+      <c r="M145" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="N145" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O145" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>146</v>
+      </c>
+      <c r="B146" t="s">
+        <v>129</v>
+      </c>
+      <c r="C146" t="s">
+        <v>141</v>
+      </c>
+      <c r="D146" t="s">
+        <v>234</v>
+      </c>
+      <c r="E146" t="s">
+        <v>152</v>
+      </c>
+      <c r="F146">
+        <f>5*0.3048</f>
+        <v>1.524</v>
+      </c>
+      <c r="G146">
+        <f>10*0.3048</f>
+        <v>3.048</v>
+      </c>
+      <c r="H146" t="s">
+        <v>38</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J146" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="K146" s="3"/>
+      <c r="L146" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M146" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N146" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O146" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>129</v>
+      </c>
+      <c r="C147" t="s">
+        <v>141</v>
+      </c>
+      <c r="D147" t="s">
+        <v>234</v>
+      </c>
+      <c r="E147" t="s">
+        <v>155</v>
+      </c>
+      <c r="F147">
+        <f>10*0.3048</f>
+        <v>3.048</v>
+      </c>
+      <c r="G147">
+        <f>15*0.3048</f>
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="H147" t="s">
+        <v>38</v>
+      </c>
+      <c r="I147" s="3">
+        <v>0</v>
+      </c>
+      <c r="J147" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K147" s="3">
+        <v>70</v>
+      </c>
+      <c r="L147" s="4">
+        <v>1</v>
+      </c>
+      <c r="M147" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="N147" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O147" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>146</v>
+      </c>
+      <c r="B148" t="s">
+        <v>129</v>
+      </c>
+      <c r="C148" t="s">
+        <v>141</v>
+      </c>
+      <c r="D148" t="s">
+        <v>234</v>
+      </c>
+      <c r="E148" t="s">
+        <v>155</v>
+      </c>
+      <c r="F148">
+        <f>10*0.3048</f>
+        <v>3.048</v>
+      </c>
+      <c r="G148">
+        <f>15*0.3048</f>
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="H148" t="s">
+        <v>38</v>
+      </c>
+      <c r="I148" s="3">
+        <v>70</v>
+      </c>
+      <c r="J148" s="3">
+        <f t="shared" si="12"/>
+        <v>70</v>
+      </c>
+      <c r="K148" s="3">
+        <v>100000</v>
+      </c>
+      <c r="L148" s="4">
+        <v>5</v>
+      </c>
+      <c r="M148" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="N148" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O148" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>146</v>
+      </c>
+      <c r="B149" t="s">
+        <v>129</v>
+      </c>
+      <c r="C149" t="s">
+        <v>141</v>
+      </c>
+      <c r="D149" t="s">
+        <v>234</v>
+      </c>
+      <c r="E149" t="s">
+        <v>155</v>
+      </c>
+      <c r="F149">
+        <f>10*0.3048</f>
+        <v>3.048</v>
+      </c>
+      <c r="G149">
+        <f>15*0.3048</f>
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="H149" t="s">
+        <v>38</v>
+      </c>
+      <c r="I149" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J149" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="K149" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L149" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M149" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N149" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O149" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>146</v>
+      </c>
+      <c r="B150" t="s">
+        <v>129</v>
+      </c>
+      <c r="C150" t="s">
+        <v>141</v>
+      </c>
+      <c r="D150" t="s">
+        <v>234</v>
+      </c>
+      <c r="E150" t="s">
+        <v>158</v>
+      </c>
+      <c r="F150">
+        <f>15*0.3048</f>
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="G150">
+        <f>20*0.3048</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="H150" t="s">
+        <v>38</v>
+      </c>
+      <c r="I150" s="3">
+        <v>0</v>
+      </c>
+      <c r="J150" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K150" s="3">
+        <v>55</v>
+      </c>
+      <c r="L150" s="4">
+        <v>1</v>
+      </c>
+      <c r="M150" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="N150" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O150" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>146</v>
+      </c>
+      <c r="B151" t="s">
+        <v>129</v>
+      </c>
+      <c r="C151" t="s">
+        <v>141</v>
+      </c>
+      <c r="D151" t="s">
+        <v>234</v>
+      </c>
+      <c r="E151" t="s">
+        <v>158</v>
+      </c>
+      <c r="F151">
+        <f>15*0.3048</f>
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="G151">
+        <f>20*0.3048</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="H151" t="s">
+        <v>38</v>
+      </c>
+      <c r="I151" s="3">
+        <v>55</v>
+      </c>
+      <c r="J151" s="3">
+        <f t="shared" si="12"/>
+        <v>55</v>
+      </c>
+      <c r="K151" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L151" s="4">
+        <v>5</v>
+      </c>
+      <c r="M151" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="N151" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O151" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>146</v>
+      </c>
+      <c r="B152" t="s">
+        <v>129</v>
+      </c>
+      <c r="C152" t="s">
+        <v>141</v>
+      </c>
+      <c r="D152" t="s">
+        <v>234</v>
+      </c>
+      <c r="E152" t="s">
+        <v>158</v>
+      </c>
+      <c r="F152">
+        <f>15*0.3048</f>
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="G152">
+        <f>20*0.3048</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="H152" t="s">
+        <v>38</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J152" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="K152" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L152" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M152" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N152" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O152" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>146</v>
+      </c>
+      <c r="B153" t="s">
+        <v>129</v>
+      </c>
+      <c r="C153" t="s">
+        <v>141</v>
+      </c>
+      <c r="D153" t="s">
+        <v>234</v>
+      </c>
+      <c r="E153" t="s">
+        <v>161</v>
+      </c>
+      <c r="F153">
+        <f>20*0.3048</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="G153">
+        <f>25*0.3048</f>
+        <v>7.62</v>
+      </c>
+      <c r="H153" t="s">
+        <v>38</v>
+      </c>
+      <c r="I153" s="3">
+        <v>0</v>
+      </c>
+      <c r="J153" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K153" s="3">
+        <v>47</v>
+      </c>
+      <c r="L153" s="4">
+        <v>1</v>
+      </c>
+      <c r="M153" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="N153" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O153" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>146</v>
+      </c>
+      <c r="B154" t="s">
+        <v>129</v>
+      </c>
+      <c r="C154" t="s">
+        <v>141</v>
+      </c>
+      <c r="D154" t="s">
+        <v>234</v>
+      </c>
+      <c r="E154" t="s">
+        <v>161</v>
+      </c>
+      <c r="F154">
+        <f>20*0.3048</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="G154">
+        <f>25*0.3048</f>
+        <v>7.62</v>
+      </c>
+      <c r="H154" t="s">
+        <v>38</v>
+      </c>
+      <c r="I154" s="3">
+        <v>47</v>
+      </c>
+      <c r="J154" s="3">
+        <f t="shared" si="12"/>
+        <v>47</v>
+      </c>
+      <c r="K154" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L154" s="4">
+        <v>5</v>
+      </c>
+      <c r="M154" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="N154" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O154" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>146</v>
+      </c>
+      <c r="B155" t="s">
+        <v>129</v>
+      </c>
+      <c r="C155" t="s">
+        <v>141</v>
+      </c>
+      <c r="D155" t="s">
+        <v>234</v>
+      </c>
+      <c r="E155" t="s">
+        <v>161</v>
+      </c>
+      <c r="F155">
+        <f>20*0.3048</f>
+        <v>6.0960000000000001</v>
+      </c>
+      <c r="G155">
+        <f>25*0.3048</f>
+        <v>7.62</v>
+      </c>
+      <c r="H155" t="s">
+        <v>38</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J155" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="K155" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L155" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M155" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N155" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O155" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>146</v>
+      </c>
+      <c r="B156" t="s">
+        <v>129</v>
+      </c>
+      <c r="C156" t="s">
+        <v>141</v>
+      </c>
+      <c r="D156" t="s">
+        <v>234</v>
+      </c>
+      <c r="E156" t="s">
+        <v>164</v>
+      </c>
+      <c r="F156">
+        <f>25*0.3048</f>
+        <v>7.62</v>
+      </c>
+      <c r="G156">
+        <f>50*0.3048</f>
+        <v>15.24</v>
+      </c>
+      <c r="H156" t="s">
+        <v>38</v>
+      </c>
+      <c r="I156" s="3">
+        <v>0</v>
+      </c>
+      <c r="J156" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K156" s="3">
+        <v>25</v>
+      </c>
+      <c r="L156" s="4">
+        <v>1</v>
+      </c>
+      <c r="M156" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N156" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O156" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>146</v>
+      </c>
+      <c r="B157" t="s">
+        <v>129</v>
+      </c>
+      <c r="C157" t="s">
+        <v>141</v>
+      </c>
+      <c r="D157" t="s">
+        <v>234</v>
+      </c>
+      <c r="E157" t="s">
+        <v>164</v>
+      </c>
+      <c r="F157">
+        <f>25*0.3048</f>
+        <v>7.62</v>
+      </c>
+      <c r="G157">
+        <f>50*0.3048</f>
+        <v>15.24</v>
+      </c>
+      <c r="H157" t="s">
+        <v>38</v>
+      </c>
+      <c r="I157" s="3">
+        <v>25</v>
+      </c>
+      <c r="J157" s="3">
+        <f t="shared" si="12"/>
+        <v>25</v>
+      </c>
+      <c r="K157" s="3">
+        <v>100000</v>
+      </c>
+      <c r="L157" s="4">
+        <v>5</v>
+      </c>
+      <c r="M157" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="N157" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O157" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>146</v>
+      </c>
+      <c r="B158" t="s">
+        <v>129</v>
+      </c>
+      <c r="C158" t="s">
+        <v>141</v>
+      </c>
+      <c r="D158" t="s">
+        <v>234</v>
+      </c>
+      <c r="E158" t="s">
+        <v>164</v>
+      </c>
+      <c r="F158">
+        <f>25*0.3048</f>
+        <v>7.62</v>
+      </c>
+      <c r="G158">
+        <f>50*0.3048</f>
+        <v>15.24</v>
+      </c>
+      <c r="H158" t="s">
+        <v>38</v>
+      </c>
+      <c r="I158" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J158" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="K158" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L158" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M158" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N158" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O158" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>146</v>
+      </c>
+      <c r="B159" t="s">
+        <v>129</v>
+      </c>
+      <c r="C159" t="s">
+        <v>141</v>
+      </c>
+      <c r="D159" t="s">
+        <v>234</v>
+      </c>
+      <c r="E159" t="s">
+        <v>167</v>
+      </c>
+      <c r="F159">
+        <f>50*0.3048</f>
+        <v>15.24</v>
+      </c>
+      <c r="G159">
+        <f>75*0.3048</f>
+        <v>22.86</v>
+      </c>
+      <c r="H159" t="s">
+        <v>38</v>
+      </c>
+      <c r="I159" s="3">
+        <v>0</v>
+      </c>
+      <c r="J159" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K159" s="3">
+        <v>23</v>
+      </c>
+      <c r="L159" s="4">
+        <v>1</v>
+      </c>
+      <c r="M159" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N159" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O159" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>146</v>
+      </c>
+      <c r="B160" t="s">
+        <v>129</v>
+      </c>
+      <c r="C160" t="s">
+        <v>141</v>
+      </c>
+      <c r="D160" t="s">
+        <v>234</v>
+      </c>
+      <c r="E160" t="s">
+        <v>167</v>
+      </c>
+      <c r="F160">
+        <f>50*0.3048</f>
+        <v>15.24</v>
+      </c>
+      <c r="G160">
+        <f>75*0.3048</f>
+        <v>22.86</v>
+      </c>
+      <c r="H160" t="s">
+        <v>38</v>
+      </c>
+      <c r="I160" s="3">
+        <v>23</v>
+      </c>
+      <c r="J160" s="3">
+        <f t="shared" si="12"/>
+        <v>23</v>
+      </c>
+      <c r="K160" s="3">
+        <v>100000</v>
+      </c>
+      <c r="L160" s="4">
+        <v>5</v>
+      </c>
+      <c r="M160" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N160" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O160" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>146</v>
+      </c>
+      <c r="B161" t="s">
+        <v>129</v>
+      </c>
+      <c r="C161" t="s">
+        <v>141</v>
+      </c>
+      <c r="D161" t="s">
+        <v>234</v>
+      </c>
+      <c r="E161" t="s">
+        <v>167</v>
+      </c>
+      <c r="F161">
+        <f>50*0.3048</f>
+        <v>15.24</v>
+      </c>
+      <c r="G161">
+        <f>75*0.3048</f>
+        <v>22.86</v>
+      </c>
+      <c r="H161" t="s">
+        <v>38</v>
+      </c>
+      <c r="I161" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J161" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="K161" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L161" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M161" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N161" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O161" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>146</v>
+      </c>
+      <c r="B162" t="s">
+        <v>129</v>
+      </c>
+      <c r="C162" t="s">
+        <v>141</v>
+      </c>
+      <c r="D162" t="s">
+        <v>234</v>
+      </c>
+      <c r="E162" t="s">
+        <v>170</v>
+      </c>
+      <c r="F162">
+        <f>75*0.3048</f>
+        <v>22.86</v>
+      </c>
+      <c r="G162">
+        <v>100000</v>
+      </c>
+      <c r="H162" t="s">
+        <v>38</v>
+      </c>
+      <c r="I162" s="3">
+        <v>0</v>
+      </c>
+      <c r="J162" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K162" s="3">
+        <v>18</v>
+      </c>
+      <c r="L162" s="4">
+        <v>1</v>
+      </c>
+      <c r="M162" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="N162" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O162" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>146</v>
+      </c>
+      <c r="B163" t="s">
+        <v>129</v>
+      </c>
+      <c r="C163" t="s">
+        <v>141</v>
+      </c>
+      <c r="D163" t="s">
+        <v>234</v>
+      </c>
+      <c r="E163" t="s">
+        <v>170</v>
+      </c>
+      <c r="F163">
+        <f>75*0.3048</f>
+        <v>22.86</v>
+      </c>
+      <c r="G163">
+        <v>100000</v>
+      </c>
+      <c r="H163" t="s">
+        <v>38</v>
+      </c>
+      <c r="I163" s="3">
+        <v>18</v>
+      </c>
+      <c r="J163" s="3">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="K163" s="3">
+        <v>100000</v>
+      </c>
+      <c r="L163" s="4">
+        <v>5</v>
+      </c>
+      <c r="M163" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="N163" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O163" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>146</v>
+      </c>
+      <c r="B164" t="s">
+        <v>129</v>
+      </c>
+      <c r="C164" t="s">
+        <v>141</v>
+      </c>
+      <c r="D164" t="s">
+        <v>234</v>
+      </c>
+      <c r="E164" t="s">
+        <v>170</v>
+      </c>
+      <c r="F164">
+        <f>75*0.3048</f>
+        <v>22.86</v>
+      </c>
+      <c r="G164">
+        <v>100000</v>
+      </c>
+      <c r="H164" t="s">
+        <v>38</v>
+      </c>
+      <c r="I164" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J164" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="K164" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L164" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M164" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N164" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O164" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:O122" xr:uid="{1E9C2260-2CB8-447D-8A92-7DAF23E0141C}"/>
-  <conditionalFormatting sqref="L2:L122">
+  <conditionalFormatting sqref="L2:L164">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>